<commit_message>
Fixing unimportant integration issues
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands.xlsx
+++ b/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Categories" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CategoriesMapping" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CodeHierarchies" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CodeHierarchiesMapping" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="DatasetQry ds1" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="DatasetQry ds2" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -1316,12 +1316,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1527,8 +1527,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1540,8 +1540,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3031,8 +3031,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>